<commit_message>
Improving Daftar Jual Saya and Search Product feature
</commit_message>
<xml_diff>
--- a/Data Files/SearchDataFiles.xlsx
+++ b/Data Files/SearchDataFiles.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Binar\Training\Katalon\binarqa-group1-web\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B1CB2124-4DA6-48FD-AF0F-4C5D4B8D4FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0281F982-DDE5-4192-9B87-21503FC175AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{A8DD1F8C-B19C-4B96-B6A9-689E515E423A}"/>
   </bookViews>
@@ -41,13 +41,13 @@
     <t>text</t>
   </si>
   <si>
-    <t>laptop</t>
+    <t>hrv</t>
   </si>
   <si>
-    <t>kemeja</t>
+    <t>flanel</t>
   </si>
   <si>
-    <t>bola</t>
+    <t>zenbook</t>
   </si>
 </sst>
 </file>
@@ -402,7 +402,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -414,7 +414,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
@@ -424,7 +424,7 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>